<commit_message>
feat: dynamic wall analysis added, in sap and abaqus, sap only lineaar
</commit_message>
<xml_diff>
--- a/comparison/3d-2side-dynamic-inelastic.xlsx
+++ b/comparison/3d-2side-dynamic-inelastic.xlsx
@@ -169,6 +169,76 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fa-IR" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+                <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+              </a:rPr>
+              <a:t>جابه جایی گره 1 در جهت </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+                <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+              </a:rPr>
+              <a:t>x</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+              <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -190,7 +260,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -542,7 +612,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -3587,11 +3657,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="333031576"/>
-        <c:axId val="333030008"/>
+        <c:axId val="322736544"/>
+        <c:axId val="327547576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="333031576"/>
+        <c:axId val="322736544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3611,6 +3681,79 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr rtl="1">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fa-IR" sz="1100">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>زمان (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>s</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fa-IR" sz="1100">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100">
+                  <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr rtl="1">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3648,12 +3791,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333030008"/>
+        <c:crossAx val="327547576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="333030008"/>
+        <c:axId val="327547576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3673,6 +3816,83 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fa-IR" sz="1100" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>جابه جایی (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>m</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fa-IR" sz="1100" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="600">
+                  <a:effectLst/>
+                  <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3710,7 +3930,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333031576"/>
+        <c:crossAx val="322736544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3722,6 +3942,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3773,6 +4025,76 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fa-IR" sz="1200" b="0" i="0" baseline="0">
+                <a:effectLst/>
+                <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+              </a:rPr>
+              <a:t>جابه جایی گره 3 در جهت </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
+                <a:effectLst/>
+                <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+              </a:rPr>
+              <a:t>x</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1050">
+              <a:effectLst/>
+              <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -3794,7 +4116,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -4146,7 +4468,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -7191,11 +7513,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="377507360"/>
-        <c:axId val="377510496"/>
+        <c:axId val="327554632"/>
+        <c:axId val="327549144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="377507360"/>
+        <c:axId val="327554632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7215,6 +7537,79 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr rtl="1">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fa-IR" sz="1100">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>زمان (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>s</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fa-IR" sz="1100">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100">
+                  <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr rtl="1">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7252,12 +7647,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="377510496"/>
+        <c:crossAx val="327549144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="377510496"/>
+        <c:axId val="327549144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7277,6 +7672,85 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr rtl="1">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fa-IR" sz="1100">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>جابه جایی</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fa-IR" sz="1100" baseline="0">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t> (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" baseline="0">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>m</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fa-IR" sz="1100" baseline="0">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100">
+                  <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr rtl="1">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7314,7 +7788,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="377507360"/>
+        <c:crossAx val="327554632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7326,6 +7800,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -10795,11 +11301,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="377510888"/>
-        <c:axId val="376824616"/>
+        <c:axId val="327547184"/>
+        <c:axId val="327549928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="377510888"/>
+        <c:axId val="327547184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10856,12 +11362,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376824616"/>
+        <c:crossAx val="327549928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="376824616"/>
+        <c:axId val="327549928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10918,7 +11424,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="377510888"/>
+        <c:crossAx val="327547184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14399,11 +14905,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="379258984"/>
-        <c:axId val="379261728"/>
+        <c:axId val="327551888"/>
+        <c:axId val="327551104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="379258984"/>
+        <c:axId val="327551888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14460,12 +14966,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379261728"/>
+        <c:crossAx val="327551104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="379261728"/>
+        <c:axId val="327551104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14522,7 +15028,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379258984"/>
+        <c:crossAx val="327551888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18035,11 +18541,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="375600528"/>
-        <c:axId val="375600136"/>
+        <c:axId val="327552672"/>
+        <c:axId val="327162432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="375600528"/>
+        <c:axId val="327552672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18096,12 +18602,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375600136"/>
+        <c:crossAx val="327162432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="375600136"/>
+        <c:axId val="327162432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18158,7 +18664,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375600528"/>
+        <c:crossAx val="327552672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -21671,11 +22177,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="379262120"/>
-        <c:axId val="379261336"/>
+        <c:axId val="327160472"/>
+        <c:axId val="327165176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="379262120"/>
+        <c:axId val="327160472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21732,12 +22238,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379261336"/>
+        <c:crossAx val="327165176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="379261336"/>
+        <c:axId val="327165176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21794,7 +22300,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379262120"/>
+        <c:crossAx val="327160472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -25256,8 +25762,8 @@
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>161192</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
@@ -25715,7 +26221,7 @@
   <dimension ref="A1:D502"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30061,8 +30567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D502"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="D4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>